<commit_message>
working on thesis, debuging all programs
</commit_message>
<xml_diff>
--- a/Code/iris detection/results/LPW_2_10.xlsx
+++ b/Code/iris detection/results/LPW_2_10.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
   <si>
     <t>frame number</t>
   </si>
@@ -40,7 +40,70 @@
     <t>(379, 264)</t>
   </si>
   <si>
-    <t>(373, 266)</t>
+    <t>(380, 264)</t>
+  </si>
+  <si>
+    <t>(381, 266)</t>
+  </si>
+  <si>
+    <t>(382, 266)</t>
+  </si>
+  <si>
+    <t>(380, 265)</t>
+  </si>
+  <si>
+    <t>(381, 263)</t>
+  </si>
+  <si>
+    <t>(382, 263)</t>
+  </si>
+  <si>
+    <t>(383, 263)</t>
+  </si>
+  <si>
+    <t>(384, 264)</t>
+  </si>
+  <si>
+    <t>(383, 264)</t>
+  </si>
+  <si>
+    <t>(382, 264)</t>
+  </si>
+  <si>
+    <t>(382, 265)</t>
+  </si>
+  <si>
+    <t>(380, 266)</t>
+  </si>
+  <si>
+    <t>(353, 235)</t>
+  </si>
+  <si>
+    <t>(369, 263)</t>
+  </si>
+  <si>
+    <t>(379, 267)</t>
+  </si>
+  <si>
+    <t>(390, 235)</t>
+  </si>
+  <si>
+    <t>(379, 265)</t>
+  </si>
+  <si>
+    <t>(368, 262)</t>
+  </si>
+  <si>
+    <t>(366, 260)</t>
+  </si>
+  <si>
+    <t>(390, 234)</t>
+  </si>
+  <si>
+    <t>(374, 263)</t>
+  </si>
+  <si>
+    <t>(367, 259)</t>
   </si>
 </sst>
 </file>
@@ -398,7 +461,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -435,19 +498,387 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1.414213562373095</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>6.324555320336759</v>
-      </c>
-      <c r="F2">
-        <v>-6</v>
-      </c>
-      <c r="G2">
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3">
         <v>2</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>41.77319714841084</v>
+      </c>
+      <c r="F4">
+        <v>-28</v>
+      </c>
+      <c r="G4">
+        <v>-31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>13.34166406412633</v>
+      </c>
+      <c r="F5">
+        <v>-13</v>
+      </c>
+      <c r="G5">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>2.23606797749979</v>
+      </c>
+      <c r="F6">
+        <v>-2</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>31.62277660168379</v>
+      </c>
+      <c r="F7">
+        <v>10</v>
+      </c>
+      <c r="G7">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1.414213562373095</v>
+      </c>
+      <c r="F8">
+        <v>-1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>2.23606797749979</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>12.16552506059644</v>
+      </c>
+      <c r="F10">
+        <v>-12</v>
+      </c>
+      <c r="G10">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" t="b">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>15.29705854077836</v>
+      </c>
+      <c r="F11">
+        <v>-15</v>
+      </c>
+      <c r="G11">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" t="b">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>2.23606797749979</v>
+      </c>
+      <c r="F12">
+        <v>-2</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>29.8328677803526</v>
+      </c>
+      <c r="F13">
+        <v>7</v>
+      </c>
+      <c r="G13">
+        <v>-29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" t="b">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>15.03329637837291</v>
+      </c>
+      <c r="F14">
+        <v>-15</v>
+      </c>
+      <c r="G14">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" t="b">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>9.055385138137417</v>
+      </c>
+      <c r="F15">
+        <v>-9</v>
+      </c>
+      <c r="G15">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>16.76305461424021</v>
+      </c>
+      <c r="F16">
+        <v>-16</v>
+      </c>
+      <c r="G16">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" t="b">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>14.14213562373095</v>
+      </c>
+      <c r="F17">
+        <v>-14</v>
+      </c>
+      <c r="G17">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" t="b">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>2.23606797749979</v>
+      </c>
+      <c r="F18">
+        <v>-2</v>
+      </c>
+      <c r="G18">
+        <v>-1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>